<commit_message>
update code submission S
</commit_message>
<xml_diff>
--- a/11-Submissions/S/dataset_1.xlsx
+++ b/11-Submissions/S/dataset_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\perso\11-Submissions\S\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E946A8A4-18D3-45C6-8245-0279EF02FF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F9F23C-EB51-4D62-86D8-90293743AEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Copy of DATASET1_2021" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="save_forecast" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'analyze&amp;forecast'!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'analyze&amp;forecast'!$A$1:$I$469</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Copy of DATASET1_2021'!$A$1:$D$253</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">save_forecast!$A$1:$G$217</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="32" r:id="rId4"/>
-    <pivotCache cacheId="33" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="10" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2686" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2699" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -138,9 +138,6 @@
   </si>
   <si>
     <t>repetitive pattern: 2 equal values then a 1 step of one</t>
-  </si>
-  <si>
-    <t>(All)</t>
   </si>
   <si>
     <t>Sum of Intake</t>
@@ -220,6 +217,9 @@
   <si>
     <t>Months (Date)</t>
   </si>
+  <si>
+    <t>(All)</t>
+  </si>
 </sst>
 </file>
 
@@ -288,15 +288,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -304,11 +310,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -321,14 +336,101 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" pivotButton="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="4" tint="0.79998168889431442"/>
@@ -341,6 +443,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF97E199"/>
+      <color rgb="FFACCCB8"/>
+      <color rgb="FF39B95B"/>
+      <color rgb="FFCDACE6"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -377,7 +487,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Demand of Product (All) in (All)</c:v>
+              <c:v>Intake Product C in all markets</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -386,8 +496,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.300855766663223"/>
-          <c:y val="4.1340418378725388E-2"/>
+          <c:x val="0.34330666771752838"/>
+          <c:y val="5.1146368138806499E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -651,6 +761,42 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -671,17 +817,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -875,88 +1010,88 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>321</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>257</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>275</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>333</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>722</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>857</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>332</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>282</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>298</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>358</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>759</c:v>
+                  <c:v>111</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1081</c:v>
+                  <c:v>113</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>371</c:v>
+                  <c:v>114</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>305</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>324</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>384</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>796</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>932</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>381</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>331</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>349</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>409</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>833</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1153</c:v>
+                  <c:v>129</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>420</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>356</c:v>
+                  <c:v>132</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>374</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>432</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -983,16 +1118,14 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln>
               <a:solidFill>
-                <a:schemeClr val="accent4">
+                <a:schemeClr val="accent1">
                   <a:lumMod val="40000"/>
                   <a:lumOff val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -1187,76 +1320,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="28">
-                  <c:v>868</c:v>
+                  <c:v>136</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1006</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>432</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>382</c:v>
+                  <c:v>141</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>399</c:v>
+                  <c:v>142</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>458</c:v>
+                  <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>906</c:v>
+                  <c:v>144</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1228</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>471</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>406</c:v>
+                  <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>423</c:v>
+                  <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>482</c:v>
+                  <c:v>151</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>942</c:v>
+                  <c:v>153</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1081</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>482</c:v>
+                  <c:v>156</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>431</c:v>
+                  <c:v>157</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>449</c:v>
+                  <c:v>158</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>509</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>980</c:v>
+                  <c:v>161</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1302</c:v>
+                  <c:v>163</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>520</c:v>
+                  <c:v>163</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>456</c:v>
+                  <c:v>165</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>474</c:v>
+                  <c:v>166</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>533</c:v>
+                  <c:v>168</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1264,7 +1397,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-1BA5-4771-9A35-87325C0E8380}"/>
+              <c16:uniqueId val="{00000001-80C8-473E-974F-86B5CAF9F812}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1377,37 +1510,6 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="bg2">
-              <a:lumMod val="95000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -1432,7 +1534,6 @@
   <c:extLst>
     <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
       <c14:pivotOptions>
-        <c14:dropZoneFilter val="1"/>
         <c14:dropZonesVisible val="1"/>
       </c14:pivotOptions>
     </c:ext>
@@ -1465,7 +1566,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>2020 vs 2021 Demand of Product B in GB</c:v>
+              <c:v>2020 vs 2021 Intake of Product C in all countries</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -1859,40 +1960,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>123</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>164</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>128</c:v>
+                  <c:v>111</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>189</c:v>
+                  <c:v>113</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1984,40 +2085,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>114</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>133</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>174</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>138</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>198</c:v>
+                  <c:v>129</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2218,8 +2319,607 @@
     <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
       <c14:pivotOptions>
         <c14:dropZoneFilter val="1"/>
-        <c14:dropZonesVisible val="1"/>
       </c14:pivotOptions>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[dataset_1.xlsx]analyze&amp;forecast!PivotTable6</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>% of Intake across per Market</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:numFmt formatCode="0%" sourceLinked="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:numFmt formatCode="0%" sourceLinked="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:numFmt formatCode="0%" sourceLinked="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="97E199"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:numFmt formatCode="0%" sourceLinked="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'analyze&amp;forecast'!$AF$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="97E199"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="0%" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'analyze&amp;forecast'!$AE$10:$AE$22</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="9"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>CA</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>GB</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>US</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>CA</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>GB</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>US</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>CA</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>GB</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>US</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>A</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>B</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>C</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'analyze&amp;forecast'!$AF$10:$AF$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>7.3266992747512222E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1941642772811604</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.23143869117895091</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3207960870298534E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.9492325855962215E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.15543936582897622</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6630123123629617E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.10595378647326699</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.11040647664024288</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-F50F-4C23-8AA8-64A1A79FE894}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1570026624"/>
+        <c:axId val="1570026144"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1570026624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1570026144"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1570026144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1570026624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
     </c:ext>
   </c:extLst>
 </c:chartSpace>
@@ -2811,13 +3511,13 @@
       <xdr:col>17</xdr:col>
       <xdr:colOff>542192</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>112346</xdr:rowOff>
+      <xdr:rowOff>144096</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>322383</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>4885</xdr:rowOff>
+      <xdr:rowOff>36635</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2837,6 +3537,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77943A82-3691-D0F1-BBDE-55BAE48AD247}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -12437,23 +13173,125 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7663B804-498C-433E-9DA5-1D28DA8A11DC}" name="PivotTable8" cacheId="33" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D854549B-FC3E-4DE8-AA40-7EFBCAE5A96B}" name="PivotTable6" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="AE9:AF22" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="13">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Intake" fld="3" showDataAs="percentOfTotal" baseField="2" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7663B804-498C-433E-9DA5-1D28DA8A11DC}" name="PivotTable8" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="S33:V47" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField numFmtId="164" showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
       <items count="4">
-        <item h="1" x="0"/>
+        <item x="0"/>
         <item x="1"/>
-        <item h="1" x="2"/>
+        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
       <items count="4">
         <item h="1" x="0"/>
-        <item x="1"/>
-        <item h="1" x="2"/>
+        <item h="1" x="1"/>
+        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -12643,8 +13481,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C229DAD1-A854-402B-BF16-92EA2DE30FB2}" name="PivotTable5" cacheId="32" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="5">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C229DAD1-A854-402B-BF16-92EA2DE30FB2}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="K35:N89" firstHeaderRow="1" firstDataRow="2" firstDataCol="2" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="10">
     <pivotField compact="0" numFmtId="164" outline="0" showAll="0">
@@ -12714,8 +13552,8 @@
     </pivotField>
     <pivotField axis="axisPage" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0">
       <items count="4">
-        <item x="0"/>
-        <item x="1"/>
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
         <item x="2"/>
         <item t="default"/>
       </items>
@@ -12723,7 +13561,7 @@
     <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
     <pivotField compact="0" outline="0" showAll="0"/>
     <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField axis="axisCol" compact="0" outline="0" showAll="0">
+    <pivotField axis="axisCol" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0">
       <items count="3">
         <item x="0"/>
         <item x="1"/>
@@ -12961,27 +13799,24 @@
     <dataField name="Sum of Intake" fld="3" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="1">
+    <format dxfId="16">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="0">
+    <format dxfId="17">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
   </formats>
   <chartFormats count="2">
-    <chartFormat chart="0" format="7" series="1">
+    <chartFormat chart="0" format="9" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
+        <references count="1">
           <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="6" count="1" selected="0">
             <x v="0"/>
           </reference>
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="8" series="1">
+    <chartFormat chart="0" format="10" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -13209,7 +14044,7 @@
   </sheetPr>
   <dimension ref="A1:D841"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -18527,11 +19362,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CC22ECB-9A98-42F4-818E-0F67015817CC}">
-  <dimension ref="A1:V469"/>
+  <dimension ref="A1:AF469"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S6" sqref="S6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -18545,19 +19380,24 @@
     <col min="11" max="11" width="12.81640625" customWidth="1"/>
     <col min="12" max="12" width="15.36328125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="40.08984375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="13" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="15.90625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="4.81640625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="11.08984375" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="4.81640625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.7265625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="23.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -18579,11 +19419,11 @@
       <c r="G1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>47</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>48</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>2</v>
@@ -18595,7 +19435,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>43496</v>
       </c>
@@ -18630,7 +19470,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>43496</v>
       </c>
@@ -18664,7 +19504,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>43496</v>
       </c>
@@ -18698,7 +19538,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>43496</v>
       </c>
@@ -18732,7 +19572,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>43496</v>
       </c>
@@ -18766,7 +19606,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>43496</v>
       </c>
@@ -18800,7 +19640,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>43496</v>
       </c>
@@ -18834,7 +19674,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>43496</v>
       </c>
@@ -18867,8 +19707,14 @@
       <c r="M9" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="AE9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>43496</v>
       </c>
@@ -18901,8 +19747,14 @@
       <c r="M10" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="AE10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF10" s="16">
+        <v>0.49886996120762356</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>43524</v>
       </c>
@@ -18926,8 +19778,14 @@
       <c r="I11" s="9">
         <v>2019</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="AE11" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF11" s="16">
+        <v>7.3266992747512222E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>43524</v>
       </c>
@@ -18951,8 +19809,14 @@
       <c r="I12" s="9">
         <v>2019</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="AE12" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF12" s="16">
+        <v>0.1941642772811604</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>43524</v>
       </c>
@@ -18976,8 +19840,14 @@
       <c r="I13" s="9">
         <v>2019</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="AE13" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF13" s="16">
+        <v>0.23143869117895091</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>43524</v>
       </c>
@@ -19001,8 +19871,14 @@
       <c r="I14" s="9">
         <v>2019</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="AE14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF14" s="16">
+        <v>0.26813965255523697</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>43524</v>
       </c>
@@ -19026,8 +19902,14 @@
       <c r="I15" s="9">
         <v>2019</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="AE15" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF15" s="16">
+        <v>2.3207960870298534E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>43524</v>
       </c>
@@ -19051,8 +19933,14 @@
       <c r="I16" s="9">
         <v>2019</v>
       </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AE16" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF16" s="16">
+        <v>8.9492325855962215E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>43524</v>
       </c>
@@ -19076,8 +19964,14 @@
       <c r="I17" s="9">
         <v>2019</v>
       </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AE17" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF17" s="16">
+        <v>0.15543936582897622</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>43524</v>
       </c>
@@ -19101,8 +19995,14 @@
       <c r="I18" s="9">
         <v>2019</v>
       </c>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AE18" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF18" s="16">
+        <v>0.2329903862371395</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>43524</v>
       </c>
@@ -19126,8 +20026,14 @@
       <c r="I19" s="9">
         <v>2019</v>
       </c>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AE19" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF19" s="16">
+        <v>1.6630123123629617E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>43555</v>
       </c>
@@ -19151,8 +20057,14 @@
       <c r="I20" s="9">
         <v>2019</v>
       </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AE20" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF20" s="16">
+        <v>0.10595378647326699</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>43555</v>
       </c>
@@ -19176,8 +20088,14 @@
       <c r="I21" s="9">
         <v>2019</v>
       </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AE21" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF21" s="16">
+        <v>0.11040647664024288</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>43555</v>
       </c>
@@ -19201,8 +20119,14 @@
       <c r="I22" s="9">
         <v>2019</v>
       </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AE22" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF22" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>43555</v>
       </c>
@@ -19227,7 +20151,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>43555</v>
       </c>
@@ -19252,7 +20176,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>43555</v>
       </c>
@@ -19277,7 +20201,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>43555</v>
       </c>
@@ -19302,7 +20226,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>43555</v>
       </c>
@@ -19327,7 +20251,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>43555</v>
       </c>
@@ -19352,7 +20276,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>43585</v>
       </c>
@@ -19377,7 +20301,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>43585</v>
       </c>
@@ -19405,13 +20329,14 @@
         <v>2</v>
       </c>
       <c r="T30" t="s">
-        <v>6</v>
-      </c>
-      <c r="U30" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="U30" s="11" t="str">
+        <f>T30</f>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>43585</v>
       </c>
@@ -19439,17 +20364,18 @@
         <v>1</v>
       </c>
       <c r="T31" t="s">
-        <v>9</v>
-      </c>
-      <c r="U31" s="9" t="s">
-        <v>9</v>
+        <v>50</v>
+      </c>
+      <c r="U31" s="12" t="str">
+        <f>T31</f>
+        <v>(All)</v>
       </c>
       <c r="V31" t="str">
-        <f>_xlfn.CONCAT("2020 vs 2021 Demand of Product ",U30," in ",U31)</f>
-        <v>2020 vs 2021 Demand of Product B in GB</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+        <f>_xlfn.CONCAT("2020 vs 2021 Intake of Product ",U30," in all countries")</f>
+        <v>2020 vs 2021 Intake of Product C in all countries</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>43585</v>
       </c>
@@ -19477,14 +20403,14 @@
         <v>2</v>
       </c>
       <c r="L32" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="M32" s="9" t="str">
         <f>L32</f>
-        <v>(All)</v>
+        <v>C</v>
       </c>
       <c r="N32" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
@@ -19515,21 +20441,21 @@
         <v>1</v>
       </c>
       <c r="L33" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="M33" s="9" t="str">
         <f>L33</f>
         <v>(All)</v>
       </c>
       <c r="N33" s="9" t="str">
-        <f>_xlfn.CONCAT("Demand of Product ",M32," in ",M33)</f>
-        <v>Demand of Product (All) in (All)</v>
+        <f>_xlfn.CONCAT("Intake Product ",M32," in ","all markets")</f>
+        <v>Intake Product C in all markets</v>
       </c>
       <c r="S33" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="T33" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="T33" s="7" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
@@ -19557,7 +20483,7 @@
         <v>2019</v>
       </c>
       <c r="S34" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T34">
         <v>2019</v>
@@ -19566,7 +20492,7 @@
         <v>2020</v>
       </c>
       <c r="V34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
@@ -19593,24 +20519,24 @@
       <c r="I35" s="9">
         <v>2019</v>
       </c>
-      <c r="K35" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="L35" s="12"/>
-      <c r="M35" s="10" t="s">
+      <c r="K35" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L35" s="15"/>
+      <c r="M35" s="14" t="s">
         <v>12</v>
       </c>
       <c r="S35" s="8">
         <v>1</v>
       </c>
-      <c r="T35">
-        <v>0</v>
-      </c>
-      <c r="U35">
-        <v>0</v>
-      </c>
-      <c r="V35">
-        <v>0</v>
+      <c r="T35" s="13">
+        <v>98</v>
+      </c>
+      <c r="U35" s="13">
+        <v>114</v>
+      </c>
+      <c r="V35" s="13">
+        <v>212</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
@@ -19638,10 +20564,10 @@
         <v>2019</v>
       </c>
       <c r="K36" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="L36" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="L36" s="7" t="s">
-        <v>50</v>
       </c>
       <c r="M36" t="s">
         <v>11</v>
@@ -19652,14 +20578,14 @@
       <c r="S36" s="8">
         <v>2</v>
       </c>
-      <c r="T36">
-        <v>0</v>
-      </c>
-      <c r="U36">
-        <v>0</v>
-      </c>
-      <c r="V36">
-        <v>0</v>
+      <c r="T36" s="13">
+        <v>100</v>
+      </c>
+      <c r="U36" s="13">
+        <v>115</v>
+      </c>
+      <c r="V36" s="13">
+        <v>215</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
@@ -19687,25 +20613,26 @@
         <v>2019</v>
       </c>
       <c r="K37" t="s">
+        <v>28</v>
+      </c>
+      <c r="L37" t="s">
         <v>29</v>
       </c>
-      <c r="L37" t="s">
-        <v>30</v>
-      </c>
-      <c r="M37">
-        <v>321</v>
-      </c>
+      <c r="M37" s="13">
+        <v>98</v>
+      </c>
+      <c r="N37" s="13"/>
       <c r="S37" s="8">
         <v>3</v>
       </c>
-      <c r="T37">
-        <v>0</v>
-      </c>
-      <c r="U37">
-        <v>0</v>
-      </c>
-      <c r="V37">
-        <v>0</v>
+      <c r="T37" s="13">
+        <v>101</v>
+      </c>
+      <c r="U37" s="13">
+        <v>117</v>
+      </c>
+      <c r="V37" s="13">
+        <v>218</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
@@ -19733,22 +20660,23 @@
         <v>2019</v>
       </c>
       <c r="L38" t="s">
-        <v>31</v>
-      </c>
-      <c r="M38">
-        <v>257</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="M38" s="13">
+        <v>100</v>
+      </c>
+      <c r="N38" s="13"/>
       <c r="S38" s="8">
         <v>4</v>
       </c>
-      <c r="T38">
-        <v>0</v>
-      </c>
-      <c r="U38">
-        <v>0</v>
-      </c>
-      <c r="V38">
-        <v>0</v>
+      <c r="T38" s="13">
+        <v>102</v>
+      </c>
+      <c r="U38" s="13">
+        <v>119</v>
+      </c>
+      <c r="V38" s="13">
+        <v>221</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
@@ -19776,22 +20704,23 @@
         <v>2019</v>
       </c>
       <c r="L39" t="s">
-        <v>32</v>
-      </c>
-      <c r="M39">
-        <v>275</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="M39" s="13">
+        <v>101</v>
+      </c>
+      <c r="N39" s="13"/>
       <c r="S39" s="8">
         <v>5</v>
       </c>
-      <c r="T39">
-        <v>123</v>
-      </c>
-      <c r="U39">
-        <v>133</v>
-      </c>
-      <c r="V39">
-        <v>256</v>
+      <c r="T39" s="13">
+        <v>103</v>
+      </c>
+      <c r="U39" s="13">
+        <v>120</v>
+      </c>
+      <c r="V39" s="13">
+        <v>223</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
@@ -19819,22 +20748,23 @@
         <v>2019</v>
       </c>
       <c r="L40" t="s">
-        <v>33</v>
-      </c>
-      <c r="M40">
-        <v>333</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="M40" s="13">
+        <v>102</v>
+      </c>
+      <c r="N40" s="13"/>
       <c r="S40" s="8">
         <v>6</v>
       </c>
-      <c r="T40">
-        <v>164</v>
-      </c>
-      <c r="U40">
-        <v>174</v>
-      </c>
-      <c r="V40">
-        <v>338</v>
+      <c r="T40" s="13">
+        <v>105</v>
+      </c>
+      <c r="U40" s="13">
+        <v>122</v>
+      </c>
+      <c r="V40" s="13">
+        <v>227</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
@@ -19862,22 +20792,23 @@
         <v>2019</v>
       </c>
       <c r="L41" t="s">
-        <v>34</v>
-      </c>
-      <c r="M41">
-        <v>722</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="M41" s="13">
+        <v>103</v>
+      </c>
+      <c r="N41" s="13"/>
       <c r="S41" s="8">
         <v>7</v>
       </c>
-      <c r="T41">
-        <v>0</v>
-      </c>
-      <c r="U41">
-        <v>0</v>
-      </c>
-      <c r="V41">
-        <v>0</v>
+      <c r="T41" s="13">
+        <v>106</v>
+      </c>
+      <c r="U41" s="13">
+        <v>122</v>
+      </c>
+      <c r="V41" s="13">
+        <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
@@ -19905,22 +20836,23 @@
         <v>2019</v>
       </c>
       <c r="L42" t="s">
-        <v>35</v>
-      </c>
-      <c r="M42">
-        <v>857</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="M42" s="13">
+        <v>105</v>
+      </c>
+      <c r="N42" s="13"/>
       <c r="S42" s="8">
         <v>8</v>
       </c>
-      <c r="T42">
-        <v>0</v>
-      </c>
-      <c r="U42">
-        <v>0</v>
-      </c>
-      <c r="V42">
-        <v>0</v>
+      <c r="T42" s="13">
+        <v>108</v>
+      </c>
+      <c r="U42" s="13">
+        <v>124</v>
+      </c>
+      <c r="V42" s="13">
+        <v>232</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
@@ -19948,22 +20880,23 @@
         <v>2019</v>
       </c>
       <c r="L43" t="s">
-        <v>36</v>
-      </c>
-      <c r="M43">
-        <v>332</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="M43" s="13">
+        <v>106</v>
+      </c>
+      <c r="N43" s="13"/>
       <c r="S43" s="8">
         <v>9</v>
       </c>
-      <c r="T43">
-        <v>0</v>
-      </c>
-      <c r="U43">
-        <v>0</v>
-      </c>
-      <c r="V43">
-        <v>0</v>
+      <c r="T43" s="13">
+        <v>108</v>
+      </c>
+      <c r="U43" s="13">
+        <v>125</v>
+      </c>
+      <c r="V43" s="13">
+        <v>233</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
@@ -19991,22 +20924,23 @@
         <v>2019</v>
       </c>
       <c r="L44" t="s">
-        <v>37</v>
-      </c>
-      <c r="M44">
-        <v>282</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="M44" s="13">
+        <v>108</v>
+      </c>
+      <c r="N44" s="13"/>
       <c r="S44" s="8">
         <v>10</v>
       </c>
-      <c r="T44">
-        <v>0</v>
-      </c>
-      <c r="U44">
-        <v>0</v>
-      </c>
-      <c r="V44">
-        <v>0</v>
+      <c r="T44" s="13">
+        <v>110</v>
+      </c>
+      <c r="U44" s="13">
+        <v>127</v>
+      </c>
+      <c r="V44" s="13">
+        <v>237</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
@@ -20034,22 +20968,23 @@
         <v>2019</v>
       </c>
       <c r="L45" t="s">
-        <v>38</v>
-      </c>
-      <c r="M45">
-        <v>298</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="M45" s="13">
+        <v>108</v>
+      </c>
+      <c r="N45" s="13"/>
       <c r="S45" s="8">
         <v>11</v>
       </c>
-      <c r="T45">
+      <c r="T45" s="13">
+        <v>111</v>
+      </c>
+      <c r="U45" s="13">
         <v>128</v>
       </c>
-      <c r="U45">
-        <v>138</v>
-      </c>
-      <c r="V45">
-        <v>266</v>
+      <c r="V45" s="13">
+        <v>239</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
@@ -20077,22 +21012,23 @@
         <v>2019</v>
       </c>
       <c r="L46" t="s">
-        <v>39</v>
-      </c>
-      <c r="M46">
-        <v>358</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="M46" s="13">
+        <v>110</v>
+      </c>
+      <c r="N46" s="13"/>
       <c r="S46" s="8">
         <v>12</v>
       </c>
-      <c r="T46">
-        <v>189</v>
-      </c>
-      <c r="U46">
-        <v>198</v>
-      </c>
-      <c r="V46">
-        <v>387</v>
+      <c r="T46" s="13">
+        <v>113</v>
+      </c>
+      <c r="U46" s="13">
+        <v>129</v>
+      </c>
+      <c r="V46" s="13">
+        <v>242</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
@@ -20120,22 +21056,23 @@
         <v>2019</v>
       </c>
       <c r="L47" t="s">
-        <v>40</v>
-      </c>
-      <c r="M47">
-        <v>759</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="M47" s="13">
+        <v>111</v>
+      </c>
+      <c r="N47" s="13"/>
       <c r="S47" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="T47">
-        <v>604</v>
-      </c>
-      <c r="U47">
-        <v>643</v>
-      </c>
-      <c r="V47">
-        <v>1247</v>
+        <v>26</v>
+      </c>
+      <c r="T47" s="13">
+        <v>1265</v>
+      </c>
+      <c r="U47" s="13">
+        <v>1462</v>
+      </c>
+      <c r="V47" s="13">
+        <v>2727</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
@@ -20163,13 +21100,14 @@
         <v>2019</v>
       </c>
       <c r="L48" t="s">
-        <v>41</v>
-      </c>
-      <c r="M48">
-        <v>1081</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="M48" s="13">
+        <v>113</v>
+      </c>
+      <c r="N48" s="13"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>43646</v>
       </c>
@@ -20194,16 +21132,17 @@
         <v>2019</v>
       </c>
       <c r="K49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L49" t="s">
-        <v>30</v>
-      </c>
-      <c r="M49">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="M49" s="13">
+        <v>114</v>
+      </c>
+      <c r="N49" s="13"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>43646</v>
       </c>
@@ -20228,13 +21167,14 @@
         <v>2019</v>
       </c>
       <c r="L50" t="s">
-        <v>31</v>
-      </c>
-      <c r="M50">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="M50" s="13">
+        <v>115</v>
+      </c>
+      <c r="N50" s="13"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>43646</v>
       </c>
@@ -20259,13 +21199,14 @@
         <v>2019</v>
       </c>
       <c r="L51" t="s">
-        <v>32</v>
-      </c>
-      <c r="M51">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="M51" s="13">
+        <v>117</v>
+      </c>
+      <c r="N51" s="13"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>43646</v>
       </c>
@@ -20290,13 +21231,14 @@
         <v>2019</v>
       </c>
       <c r="L52" t="s">
-        <v>33</v>
-      </c>
-      <c r="M52">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="M52" s="13">
+        <v>119</v>
+      </c>
+      <c r="N52" s="13"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>43646</v>
       </c>
@@ -20321,13 +21263,14 @@
         <v>2019</v>
       </c>
       <c r="L53" t="s">
-        <v>34</v>
-      </c>
-      <c r="M53">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="M53" s="13">
+        <v>120</v>
+      </c>
+      <c r="N53" s="13"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>43646</v>
       </c>
@@ -20352,13 +21295,14 @@
         <v>2019</v>
       </c>
       <c r="L54" t="s">
-        <v>35</v>
-      </c>
-      <c r="M54">
-        <v>932</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="M54" s="13">
+        <v>122</v>
+      </c>
+      <c r="N54" s="13"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>43646</v>
       </c>
@@ -20383,13 +21327,14 @@
         <v>2019</v>
       </c>
       <c r="L55" t="s">
-        <v>36</v>
-      </c>
-      <c r="M55">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="M55" s="13">
+        <v>122</v>
+      </c>
+      <c r="N55" s="13"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>43677</v>
       </c>
@@ -20414,13 +21359,14 @@
         <v>2019</v>
       </c>
       <c r="L56" t="s">
-        <v>37</v>
-      </c>
-      <c r="M56">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="M56" s="13">
+        <v>124</v>
+      </c>
+      <c r="N56" s="13"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>43677</v>
       </c>
@@ -20445,13 +21391,14 @@
         <v>2019</v>
       </c>
       <c r="L57" t="s">
-        <v>38</v>
-      </c>
-      <c r="M57">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="M57" s="13">
+        <v>125</v>
+      </c>
+      <c r="N57" s="13"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>43677</v>
       </c>
@@ -20476,13 +21423,14 @@
         <v>2019</v>
       </c>
       <c r="L58" t="s">
-        <v>39</v>
-      </c>
-      <c r="M58">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="M58" s="13">
+        <v>127</v>
+      </c>
+      <c r="N58" s="13"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>43677</v>
       </c>
@@ -20507,13 +21455,14 @@
         <v>2019</v>
       </c>
       <c r="L59" t="s">
-        <v>40</v>
-      </c>
-      <c r="M59">
-        <v>833</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="M59" s="13">
+        <v>128</v>
+      </c>
+      <c r="N59" s="13"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>43677</v>
       </c>
@@ -20538,13 +21487,14 @@
         <v>2019</v>
       </c>
       <c r="L60" t="s">
-        <v>41</v>
-      </c>
-      <c r="M60">
-        <v>1153</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="M60" s="13">
+        <v>129</v>
+      </c>
+      <c r="N60" s="13"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>43677</v>
       </c>
@@ -20569,16 +21519,17 @@
         <v>2019</v>
       </c>
       <c r="K61" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L61" t="s">
-        <v>30</v>
-      </c>
-      <c r="M61">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="M61" s="13">
+        <v>130</v>
+      </c>
+      <c r="N61" s="13"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>43677</v>
       </c>
@@ -20603,13 +21554,14 @@
         <v>2019</v>
       </c>
       <c r="L62" t="s">
-        <v>31</v>
-      </c>
-      <c r="M62">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="M62" s="13">
+        <v>132</v>
+      </c>
+      <c r="N62" s="13"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>43677</v>
       </c>
@@ -20634,13 +21586,14 @@
         <v>2019</v>
       </c>
       <c r="L63" t="s">
-        <v>32</v>
-      </c>
-      <c r="M63">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="M63" s="13">
+        <v>133</v>
+      </c>
+      <c r="N63" s="13"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>43677</v>
       </c>
@@ -20665,11 +21618,12 @@
         <v>2019</v>
       </c>
       <c r="L64" t="s">
-        <v>33</v>
-      </c>
-      <c r="M64">
-        <v>432</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="M64" s="13">
+        <v>135</v>
+      </c>
+      <c r="N64" s="13"/>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
@@ -20696,10 +21650,11 @@
         <v>2019</v>
       </c>
       <c r="L65" t="s">
-        <v>34</v>
-      </c>
-      <c r="N65">
-        <v>868</v>
+        <v>33</v>
+      </c>
+      <c r="M65" s="13"/>
+      <c r="N65" s="13">
+        <v>136</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
@@ -20727,10 +21682,11 @@
         <v>2019</v>
       </c>
       <c r="L66" t="s">
-        <v>35</v>
-      </c>
-      <c r="N66">
-        <v>1006</v>
+        <v>34</v>
+      </c>
+      <c r="M66" s="13"/>
+      <c r="N66" s="13">
+        <v>138</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
@@ -20758,10 +21714,11 @@
         <v>2019</v>
       </c>
       <c r="L67" t="s">
-        <v>36</v>
-      </c>
-      <c r="N67">
-        <v>432</v>
+        <v>35</v>
+      </c>
+      <c r="M67" s="13"/>
+      <c r="N67" s="13">
+        <v>139</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
@@ -20789,10 +21746,11 @@
         <v>2019</v>
       </c>
       <c r="L68" t="s">
-        <v>37</v>
-      </c>
-      <c r="N68">
-        <v>382</v>
+        <v>36</v>
+      </c>
+      <c r="M68" s="13"/>
+      <c r="N68" s="13">
+        <v>141</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
@@ -20820,10 +21778,11 @@
         <v>2019</v>
       </c>
       <c r="L69" t="s">
-        <v>38</v>
-      </c>
-      <c r="N69">
-        <v>399</v>
+        <v>37</v>
+      </c>
+      <c r="M69" s="13"/>
+      <c r="N69" s="13">
+        <v>142</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
@@ -20851,10 +21810,11 @@
         <v>2019</v>
       </c>
       <c r="L70" t="s">
-        <v>39</v>
-      </c>
-      <c r="N70">
-        <v>458</v>
+        <v>38</v>
+      </c>
+      <c r="M70" s="13"/>
+      <c r="N70" s="13">
+        <v>143</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
@@ -20882,10 +21842,11 @@
         <v>2019</v>
       </c>
       <c r="L71" t="s">
-        <v>40</v>
-      </c>
-      <c r="N71">
-        <v>906</v>
+        <v>39</v>
+      </c>
+      <c r="M71" s="13"/>
+      <c r="N71" s="13">
+        <v>144</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
@@ -20913,10 +21874,11 @@
         <v>2019</v>
       </c>
       <c r="L72" t="s">
-        <v>41</v>
-      </c>
-      <c r="N72">
-        <v>1228</v>
+        <v>40</v>
+      </c>
+      <c r="M72" s="13"/>
+      <c r="N72" s="13">
+        <v>146</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
@@ -20944,13 +21906,14 @@
         <v>2019</v>
       </c>
       <c r="K73" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L73" t="s">
-        <v>30</v>
-      </c>
-      <c r="N73">
-        <v>471</v>
+        <v>29</v>
+      </c>
+      <c r="M73" s="13"/>
+      <c r="N73" s="13">
+        <v>147</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
@@ -20978,10 +21941,11 @@
         <v>2019</v>
       </c>
       <c r="L74" t="s">
-        <v>31</v>
-      </c>
-      <c r="N74">
-        <v>406</v>
+        <v>30</v>
+      </c>
+      <c r="M74" s="13"/>
+      <c r="N74" s="13">
+        <v>149</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
@@ -21009,10 +21973,11 @@
         <v>2019</v>
       </c>
       <c r="L75" t="s">
-        <v>32</v>
-      </c>
-      <c r="N75">
-        <v>423</v>
+        <v>31</v>
+      </c>
+      <c r="M75" s="13"/>
+      <c r="N75" s="13">
+        <v>149</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
@@ -21040,10 +22005,11 @@
         <v>2019</v>
       </c>
       <c r="L76" t="s">
-        <v>33</v>
-      </c>
-      <c r="N76">
-        <v>482</v>
+        <v>32</v>
+      </c>
+      <c r="M76" s="13"/>
+      <c r="N76" s="13">
+        <v>151</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
@@ -21071,10 +22037,11 @@
         <v>2019</v>
       </c>
       <c r="L77" t="s">
-        <v>34</v>
-      </c>
-      <c r="N77">
-        <v>942</v>
+        <v>33</v>
+      </c>
+      <c r="M77" s="13"/>
+      <c r="N77" s="13">
+        <v>153</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
@@ -21102,10 +22069,11 @@
         <v>2019</v>
       </c>
       <c r="L78" t="s">
-        <v>35</v>
-      </c>
-      <c r="N78">
-        <v>1081</v>
+        <v>34</v>
+      </c>
+      <c r="M78" s="13"/>
+      <c r="N78" s="13">
+        <v>155</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
@@ -21133,10 +22101,11 @@
         <v>2019</v>
       </c>
       <c r="L79" t="s">
-        <v>36</v>
-      </c>
-      <c r="N79">
-        <v>482</v>
+        <v>35</v>
+      </c>
+      <c r="M79" s="13"/>
+      <c r="N79" s="13">
+        <v>156</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.25">
@@ -21164,10 +22133,11 @@
         <v>2019</v>
       </c>
       <c r="L80" t="s">
-        <v>37</v>
-      </c>
-      <c r="N80">
-        <v>431</v>
+        <v>36</v>
+      </c>
+      <c r="M80" s="13"/>
+      <c r="N80" s="13">
+        <v>157</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
@@ -21195,10 +22165,11 @@
         <v>2019</v>
       </c>
       <c r="L81" t="s">
-        <v>38</v>
-      </c>
-      <c r="N81">
-        <v>449</v>
+        <v>37</v>
+      </c>
+      <c r="M81" s="13"/>
+      <c r="N81" s="13">
+        <v>158</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
@@ -21226,10 +22197,11 @@
         <v>2019</v>
       </c>
       <c r="L82" t="s">
-        <v>39</v>
-      </c>
-      <c r="N82">
-        <v>509</v>
+        <v>38</v>
+      </c>
+      <c r="M82" s="13"/>
+      <c r="N82" s="13">
+        <v>160</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
@@ -21257,10 +22229,11 @@
         <v>2019</v>
       </c>
       <c r="L83" t="s">
-        <v>40</v>
-      </c>
-      <c r="N83">
-        <v>980</v>
+        <v>39</v>
+      </c>
+      <c r="M83" s="13"/>
+      <c r="N83" s="13">
+        <v>161</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
@@ -21288,10 +22261,11 @@
         <v>2019</v>
       </c>
       <c r="L84" t="s">
-        <v>41</v>
-      </c>
-      <c r="N84">
-        <v>1302</v>
+        <v>40</v>
+      </c>
+      <c r="M84" s="13"/>
+      <c r="N84" s="13">
+        <v>163</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
@@ -21319,13 +22293,14 @@
         <v>2019</v>
       </c>
       <c r="K85" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L85" t="s">
-        <v>30</v>
-      </c>
-      <c r="N85">
-        <v>520</v>
+        <v>29</v>
+      </c>
+      <c r="M85" s="13"/>
+      <c r="N85" s="13">
+        <v>163</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
@@ -21353,10 +22328,11 @@
         <v>2019</v>
       </c>
       <c r="L86" t="s">
-        <v>31</v>
-      </c>
-      <c r="N86">
-        <v>456</v>
+        <v>30</v>
+      </c>
+      <c r="M86" s="13"/>
+      <c r="N86" s="13">
+        <v>165</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
@@ -21384,10 +22360,11 @@
         <v>2019</v>
       </c>
       <c r="L87" t="s">
-        <v>32</v>
-      </c>
-      <c r="N87">
-        <v>474</v>
+        <v>31</v>
+      </c>
+      <c r="M87" s="13"/>
+      <c r="N87" s="13">
+        <v>166</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
@@ -21415,10 +22392,11 @@
         <v>2019</v>
       </c>
       <c r="L88" t="s">
-        <v>33</v>
-      </c>
-      <c r="N88">
-        <v>533</v>
+        <v>32</v>
+      </c>
+      <c r="M88" s="13"/>
+      <c r="N88" s="13">
+        <v>168</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
@@ -21446,13 +22424,13 @@
         <v>2019</v>
       </c>
       <c r="K89" t="s">
-        <v>27</v>
-      </c>
-      <c r="M89">
-        <v>14025</v>
-      </c>
-      <c r="N89">
-        <v>15620</v>
+        <v>26</v>
+      </c>
+      <c r="M89" s="13">
+        <v>3257</v>
+      </c>
+      <c r="N89" s="13">
+        <v>3650</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
@@ -33476,10 +34454,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1" xr:uid="{3CC22ECB-9A98-42F4-818E-0F67015817CC}"/>
+  <autoFilter ref="A1:I469" xr:uid="{3CC22ECB-9A98-42F4-818E-0F67015817CC}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
-  <drawing r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+  <ignoredErrors>
+    <ignoredError sqref="F119 F128 F137 F146:F236 F245" formula="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>